<commit_message>
added tokenization, optimized GPT3 answer by adding a stopping sequence
</commit_message>
<xml_diff>
--- a/blueprint-primer-general-and-specific.xlsx
+++ b/blueprint-primer-general-and-specific.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">What is blueprint?</t>
   </si>
   <si>
-    <t xml:space="preserve">blueprint is a paradigm that lets you write schema code and it can generate code while at the same time giving you the ability to add features, modify code and also support additional functionalities. Because Blueprint outputs an X-Framework compatible project, it's important that you have you are up to date with the X-Framework basics. \n\n</t>
+    <t xml:space="preserve">blueprint is a paradigm that lets you write schema code and it can generate code while at the same time giving you the ability to add features, modify code and also support additional functionalities. Because Blueprint outputs an X-Framework compatible project, it's important that you are up to date with the X-Framework basics. \n\n</t>
   </si>
   <si>
     <t xml:space="preserve">Pre-requisites for building a project in blueprint:</t>
@@ -176,7 +176,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>